<commit_message>
Added a description for metadata
</commit_message>
<xml_diff>
--- a/Understanding Data/Metadata - Harwinder.xlsx
+++ b/Understanding Data/Metadata - Harwinder.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="32" documentId="11_F25DC773A252ABEACE02EC6B639863985BDE589E" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{1E46283B-2816-4FD4-A7AF-CECC63114F07}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="11_F25DC773A252ABEACE02EC6B639863985BDE589E" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{FCFF4D41-6C4B-4098-9F47-AA2C0EB4F13F}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>Comprehensive Species Tally</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Vikash, Edem, Harwinder</t>
+  </si>
+  <si>
+    <t>Data about location</t>
   </si>
 </sst>
 </file>
@@ -461,7 +464,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -516,7 +519,9 @@
       <c r="D3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>

</xml_diff>